<commit_message>
Results of second exercise
</commit_message>
<xml_diff>
--- a/Yearly Forecasting/Revenue/Yearly_Forecast_Revenue.xlsx
+++ b/Yearly Forecasting/Revenue/Yearly_Forecast_Revenue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/msramirezgo_unal_edu_co/Documents/Oliver Pardo/VAR_VEC-2023/Yearly Forecasting/Revenue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{424274BD-41AF-44B3-AD25-A9BCC47C8A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4884EB2-6164-469F-9414-1050A933A0D3}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{424274BD-41AF-44B3-AD25-A9BCC47C8A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45FEB0F4-BDD4-42F3-A3FF-D7BFC759AED6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="805" firstSheet="1" activeTab="9" xr2:uid="{486D11B9-5307-4873-8238-7EE5ADB2402D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="805" xr2:uid="{486D11B9-5307-4873-8238-7EE5ADB2402D}"/>
   </bookViews>
   <sheets>
     <sheet name="Total revenues and grants" sheetId="5" r:id="rId1"/>
@@ -140,12 +140,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -204,7 +210,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -228,6 +234,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -17735,6 +17745,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -18034,8 +18048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A81BD89-865E-4FDA-A792-CCBA127E0C69}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18429,13 +18443,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="9">
         <v>2021</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="10">
         <v>728523657.75299275</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="10">
         <v>3883368104.5708337</v>
       </c>
       <c r="D23" s="2">
@@ -18448,13 +18462,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="9">
         <v>2022</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="10">
         <v>538219822.8087101</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="10">
         <v>3921493261.8216152</v>
       </c>
       <c r="D24" s="2">
@@ -18467,13 +18481,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="9">
         <v>2023</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="10">
         <v>439647879.26706791</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="10">
         <v>4008236005.347024</v>
       </c>
       <c r="D25" s="2">
@@ -18486,13 +18500,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="9">
         <v>2024</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="10">
         <v>400707527.74236143</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="10">
         <v>4096764000.8919373</v>
       </c>
       <c r="D26" s="2">
@@ -18505,13 +18519,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="9">
         <v>2025</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="10">
         <v>383882654.2928521</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="10">
         <v>4189882842.3564558</v>
       </c>
       <c r="D27" s="2">
@@ -18534,7 +18548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263AF6BA-B4E9-40E2-8E8F-D0CA4D66AC4E}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>

</xml_diff>